<commit_message>
refactor: Se separaron las responsabilidades para entrenar el modelo y predecir
</commit_message>
<xml_diff>
--- a/data/excel/setData.xlsx
+++ b/data/excel/setData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28bf719b72b0f565/Escritorio/studentsBack-ED/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_6B2D71A5D350DA13BFD92F11595ED87656DDACA3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A2D8B16-1B10-4052-91BB-EA247101F496}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_6B2D71A5D350DA13BFD92F11595ED87656DDACA3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C026B7D9-491F-47A6-B53D-60757D366E70}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4920" yWindow="1260" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -343,6 +343,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -630,12 +634,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1941"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A427" workbookViewId="0">
-      <selection activeCell="N1" sqref="M1:N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>